<commit_message>
change base resistor(R4) from 2k4 to 1k0 Schematic & BOM was changed
</commit_message>
<xml_diff>
--- a/H0FR10/Released/BOM/H0FR10.xlsx
+++ b/H0FR10/Released/BOM/H0FR10.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\H0FR1x-Hardware\H0FR10\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK PEICE\HEXABITZ\h0fr1\H0FR10\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABF2534-7E1A-4D48-B0F6-DC100C87DA1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22695" windowHeight="14595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +25,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="H10R4" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -47,7 +46,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="2" name="H10R41" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="932" sourceFile="C:\Work\27\Asaad\Modules\H10R4\Delivery\Released\BOM\H10R4.csv" semicolon="1">
       <textFields count="14">
         <textField/>
@@ -109,9 +108,6 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
     <t>10.0K</t>
   </si>
   <si>
@@ -250,9 +246,6 @@
     <t>https://octopart.com/erj-3geyj181v-panasonic-55403673</t>
   </si>
   <si>
-    <t xml:space="preserve">https://octopart.com/crcw06032k40jnea-vishay-40298967 </t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -326,12 +319,18 @@
   </si>
   <si>
     <t>https://octopart.com/g5le-14-dc3-omron-6508769?r=sp&amp;s=6I6RsLueSo2S2OmQXlG-5Q</t>
+  </si>
+  <si>
+    <t>https://octopart.com/crcw06031k00jnea-vishay-55388219?r=sp</t>
+  </si>
+  <si>
+    <t>CRCW06031K00JNEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +426,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="H10R4" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="H10R4" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,23 +505,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -558,23 +540,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -750,34 +715,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.265625" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="60.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.59765625" customWidth="1"/>
-    <col min="8" max="8" width="6.265625" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -795,153 +760,153 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -950,13 +915,13 @@
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -964,27 +929,27 @@
         <v>180</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -996,21 +961,21 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>2400</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -1019,13 +984,13 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1033,45 +998,45 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1082,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
@@ -1094,85 +1059,85 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{F09E3B28-65A7-4690-BEC4-7EB20B057B1B}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{DE796448-EC12-43AC-BE72-57225FD1A99D}"/>
-    <hyperlink ref="G9" r:id="rId3" xr:uid="{0854D7BB-AB48-4A63-A737-C516838E4532}"/>
-    <hyperlink ref="G10" r:id="rId4" xr:uid="{A7368773-562E-4B54-9235-3E7975DFDA0A}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{655C8BFE-FFB3-498A-AD0A-70D76392BA95}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{B2EBB925-5731-4516-9128-68DFFE84B154}"/>
-    <hyperlink ref="G15" r:id="rId7" xr:uid="{2230FFF6-0283-4FF2-9A41-3FFC91DB79DE}"/>
-    <hyperlink ref="G16" r:id="rId8" xr:uid="{17ED9B62-6693-4F3F-8B74-AF2003D8D35A}"/>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+    <hyperlink ref="G10" r:id="rId4"/>
+    <hyperlink ref="G11" r:id="rId5"/>
+    <hyperlink ref="G12" r:id="rId6"/>
+    <hyperlink ref="G15" r:id="rId7"/>
+    <hyperlink ref="G16" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -1180,24 +1145,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>